<commit_message>
upando a melhor API pra covid
</commit_message>
<xml_diff>
--- a/studio/dados_Juazeiro.xlsx
+++ b/studio/dados_Juazeiro.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F361"/>
+  <dimension ref="A1:G364"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -389,6 +389,11 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
+          <t>population</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
           <t>date</t>
         </is>
       </c>
@@ -411,7 +416,10 @@
       <c r="E2" t="n">
         <v>1</v>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G2" t="inlineStr">
         <is>
           <t>23/mar</t>
         </is>
@@ -435,7 +443,10 @@
       <c r="E3" t="n">
         <v>1</v>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="F3" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G3" t="inlineStr">
         <is>
           <t>24/mar</t>
         </is>
@@ -459,7 +470,10 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="F4" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G4" t="inlineStr">
         <is>
           <t>25/mar</t>
         </is>
@@ -483,7 +497,10 @@
       <c r="E5" t="n">
         <v>0</v>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="F5" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G5" t="inlineStr">
         <is>
           <t>26/mar</t>
         </is>
@@ -507,7 +524,10 @@
       <c r="E6" t="n">
         <v>0</v>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="F6" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G6" t="inlineStr">
         <is>
           <t>27/mar</t>
         </is>
@@ -531,7 +551,10 @@
       <c r="E7" t="n">
         <v>0</v>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="F7" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G7" t="inlineStr">
         <is>
           <t>28/mar</t>
         </is>
@@ -555,7 +578,10 @@
       <c r="E8" t="n">
         <v>0</v>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="F8" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G8" t="inlineStr">
         <is>
           <t>29/mar</t>
         </is>
@@ -579,7 +605,10 @@
       <c r="E9" t="n">
         <v>0</v>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G9" t="inlineStr">
         <is>
           <t>30/mar</t>
         </is>
@@ -603,7 +632,10 @@
       <c r="E10" t="n">
         <v>0</v>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="F10" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G10" t="inlineStr">
         <is>
           <t>31/mar</t>
         </is>
@@ -627,7 +659,10 @@
       <c r="E11" t="n">
         <v>0</v>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="F11" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G11" t="inlineStr">
         <is>
           <t>01/abr</t>
         </is>
@@ -651,7 +686,10 @@
       <c r="E12" t="n">
         <v>0</v>
       </c>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>02/abr</t>
         </is>
@@ -675,7 +713,10 @@
       <c r="E13" t="n">
         <v>0</v>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="F13" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G13" t="inlineStr">
         <is>
           <t>03/abr</t>
         </is>
@@ -699,7 +740,10 @@
       <c r="E14" t="n">
         <v>0</v>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="F14" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G14" t="inlineStr">
         <is>
           <t>04/abr</t>
         </is>
@@ -723,7 +767,10 @@
       <c r="E15" t="n">
         <v>1</v>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G15" t="inlineStr">
         <is>
           <t>05/abr</t>
         </is>
@@ -747,7 +794,10 @@
       <c r="E16" t="n">
         <v>0</v>
       </c>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G16" t="inlineStr">
         <is>
           <t>06/abr</t>
         </is>
@@ -771,7 +821,10 @@
       <c r="E17" t="n">
         <v>0</v>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G17" t="inlineStr">
         <is>
           <t>07/abr</t>
         </is>
@@ -795,7 +848,10 @@
       <c r="E18" t="n">
         <v>0</v>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="F18" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G18" t="inlineStr">
         <is>
           <t>08/abr</t>
         </is>
@@ -819,7 +875,10 @@
       <c r="E19" t="n">
         <v>0</v>
       </c>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G19" t="inlineStr">
         <is>
           <t>09/abr</t>
         </is>
@@ -843,7 +902,10 @@
       <c r="E20" t="n">
         <v>0</v>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="F20" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G20" t="inlineStr">
         <is>
           <t>10/abr</t>
         </is>
@@ -867,7 +929,10 @@
       <c r="E21" t="n">
         <v>2</v>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="F21" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G21" t="inlineStr">
         <is>
           <t>11/abr</t>
         </is>
@@ -891,7 +956,10 @@
       <c r="E22" t="n">
         <v>0</v>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="F22" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G22" t="inlineStr">
         <is>
           <t>12/abr</t>
         </is>
@@ -915,7 +983,10 @@
       <c r="E23" t="n">
         <v>0</v>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F23" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G23" t="inlineStr">
         <is>
           <t>13/abr</t>
         </is>
@@ -939,7 +1010,10 @@
       <c r="E24" t="n">
         <v>0</v>
       </c>
-      <c r="F24" t="inlineStr">
+      <c r="F24" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G24" t="inlineStr">
         <is>
           <t>14/abr</t>
         </is>
@@ -963,7 +1037,10 @@
       <c r="E25" t="n">
         <v>0</v>
       </c>
-      <c r="F25" t="inlineStr">
+      <c r="F25" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G25" t="inlineStr">
         <is>
           <t>15/abr</t>
         </is>
@@ -987,7 +1064,10 @@
       <c r="E26" t="n">
         <v>0</v>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="F26" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G26" t="inlineStr">
         <is>
           <t>16/abr</t>
         </is>
@@ -1011,7 +1091,10 @@
       <c r="E27" t="n">
         <v>0</v>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="F27" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G27" t="inlineStr">
         <is>
           <t>17/abr</t>
         </is>
@@ -1035,7 +1118,10 @@
       <c r="E28" t="n">
         <v>0</v>
       </c>
-      <c r="F28" t="inlineStr">
+      <c r="F28" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G28" t="inlineStr">
         <is>
           <t>18/abr</t>
         </is>
@@ -1059,7 +1145,10 @@
       <c r="E29" t="n">
         <v>2</v>
       </c>
-      <c r="F29" t="inlineStr">
+      <c r="F29" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G29" t="inlineStr">
         <is>
           <t>19/abr</t>
         </is>
@@ -1083,7 +1172,10 @@
       <c r="E30" t="n">
         <v>0</v>
       </c>
-      <c r="F30" t="inlineStr">
+      <c r="F30" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G30" t="inlineStr">
         <is>
           <t>20/abr</t>
         </is>
@@ -1107,7 +1199,10 @@
       <c r="E31" t="n">
         <v>0</v>
       </c>
-      <c r="F31" t="inlineStr">
+      <c r="F31" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G31" t="inlineStr">
         <is>
           <t>21/abr</t>
         </is>
@@ -1131,7 +1226,10 @@
       <c r="E32" t="n">
         <v>0</v>
       </c>
-      <c r="F32" t="inlineStr">
+      <c r="F32" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G32" t="inlineStr">
         <is>
           <t>22/abr</t>
         </is>
@@ -1155,7 +1253,10 @@
       <c r="E33" t="n">
         <v>0</v>
       </c>
-      <c r="F33" t="inlineStr">
+      <c r="F33" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G33" t="inlineStr">
         <is>
           <t>23/abr</t>
         </is>
@@ -1179,7 +1280,10 @@
       <c r="E34" t="n">
         <v>0</v>
       </c>
-      <c r="F34" t="inlineStr">
+      <c r="F34" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G34" t="inlineStr">
         <is>
           <t>24/abr</t>
         </is>
@@ -1203,7 +1307,10 @@
       <c r="E35" t="n">
         <v>1</v>
       </c>
-      <c r="F35" t="inlineStr">
+      <c r="F35" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G35" t="inlineStr">
         <is>
           <t>25/abr</t>
         </is>
@@ -1227,7 +1334,10 @@
       <c r="E36" t="n">
         <v>1</v>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="F36" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G36" t="inlineStr">
         <is>
           <t>26/abr</t>
         </is>
@@ -1251,7 +1361,10 @@
       <c r="E37" t="n">
         <v>0</v>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F37" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G37" t="inlineStr">
         <is>
           <t>27/abr</t>
         </is>
@@ -1275,7 +1388,10 @@
       <c r="E38" t="n">
         <v>0</v>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="F38" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G38" t="inlineStr">
         <is>
           <t>28/abr</t>
         </is>
@@ -1299,7 +1415,10 @@
       <c r="E39" t="n">
         <v>0</v>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="F39" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G39" t="inlineStr">
         <is>
           <t>29/abr</t>
         </is>
@@ -1323,7 +1442,10 @@
       <c r="E40" t="n">
         <v>0</v>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F40" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G40" t="inlineStr">
         <is>
           <t>30/abr</t>
         </is>
@@ -1347,7 +1469,10 @@
       <c r="E41" t="n">
         <v>0</v>
       </c>
-      <c r="F41" t="inlineStr">
+      <c r="F41" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G41" t="inlineStr">
         <is>
           <t>01/mai</t>
         </is>
@@ -1371,7 +1496,10 @@
       <c r="E42" t="n">
         <v>0</v>
       </c>
-      <c r="F42" t="inlineStr">
+      <c r="F42" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G42" t="inlineStr">
         <is>
           <t>02/mai</t>
         </is>
@@ -1395,7 +1523,10 @@
       <c r="E43" t="n">
         <v>0</v>
       </c>
-      <c r="F43" t="inlineStr">
+      <c r="F43" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G43" t="inlineStr">
         <is>
           <t>03/mai</t>
         </is>
@@ -1419,7 +1550,10 @@
       <c r="E44" t="n">
         <v>0</v>
       </c>
-      <c r="F44" t="inlineStr">
+      <c r="F44" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G44" t="inlineStr">
         <is>
           <t>04/mai</t>
         </is>
@@ -1443,7 +1577,10 @@
       <c r="E45" t="n">
         <v>0</v>
       </c>
-      <c r="F45" t="inlineStr">
+      <c r="F45" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G45" t="inlineStr">
         <is>
           <t>05/mai</t>
         </is>
@@ -1467,7 +1604,10 @@
       <c r="E46" t="n">
         <v>0</v>
       </c>
-      <c r="F46" t="inlineStr">
+      <c r="F46" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G46" t="inlineStr">
         <is>
           <t>06/mai</t>
         </is>
@@ -1491,7 +1631,10 @@
       <c r="E47" t="n">
         <v>0</v>
       </c>
-      <c r="F47" t="inlineStr">
+      <c r="F47" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G47" t="inlineStr">
         <is>
           <t>07/mai</t>
         </is>
@@ -1515,7 +1658,10 @@
       <c r="E48" t="n">
         <v>0</v>
       </c>
-      <c r="F48" t="inlineStr">
+      <c r="F48" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G48" t="inlineStr">
         <is>
           <t>08/mai</t>
         </is>
@@ -1539,7 +1685,10 @@
       <c r="E49" t="n">
         <v>0</v>
       </c>
-      <c r="F49" t="inlineStr">
+      <c r="F49" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G49" t="inlineStr">
         <is>
           <t>09/mai</t>
         </is>
@@ -1563,7 +1712,10 @@
       <c r="E50" t="n">
         <v>1</v>
       </c>
-      <c r="F50" t="inlineStr">
+      <c r="F50" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G50" t="inlineStr">
         <is>
           <t>10/mai</t>
         </is>
@@ -1587,7 +1739,10 @@
       <c r="E51" t="n">
         <v>0</v>
       </c>
-      <c r="F51" t="inlineStr">
+      <c r="F51" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G51" t="inlineStr">
         <is>
           <t>11/mai</t>
         </is>
@@ -1611,7 +1766,10 @@
       <c r="E52" t="n">
         <v>2</v>
       </c>
-      <c r="F52" t="inlineStr">
+      <c r="F52" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G52" t="inlineStr">
         <is>
           <t>12/mai</t>
         </is>
@@ -1635,7 +1793,10 @@
       <c r="E53" t="n">
         <v>0</v>
       </c>
-      <c r="F53" t="inlineStr">
+      <c r="F53" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G53" t="inlineStr">
         <is>
           <t>13/mai</t>
         </is>
@@ -1659,7 +1820,10 @@
       <c r="E54" t="n">
         <v>0</v>
       </c>
-      <c r="F54" t="inlineStr">
+      <c r="F54" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G54" t="inlineStr">
         <is>
           <t>14/mai</t>
         </is>
@@ -1683,7 +1847,10 @@
       <c r="E55" t="n">
         <v>14</v>
       </c>
-      <c r="F55" t="inlineStr">
+      <c r="F55" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G55" t="inlineStr">
         <is>
           <t>15/mai</t>
         </is>
@@ -1707,7 +1874,10 @@
       <c r="E56" t="n">
         <v>0</v>
       </c>
-      <c r="F56" t="inlineStr">
+      <c r="F56" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G56" t="inlineStr">
         <is>
           <t>16/mai</t>
         </is>
@@ -1731,7 +1901,10 @@
       <c r="E57" t="n">
         <v>0</v>
       </c>
-      <c r="F57" t="inlineStr">
+      <c r="F57" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G57" t="inlineStr">
         <is>
           <t>17/mai</t>
         </is>
@@ -1755,7 +1928,10 @@
       <c r="E58" t="n">
         <v>0</v>
       </c>
-      <c r="F58" t="inlineStr">
+      <c r="F58" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G58" t="inlineStr">
         <is>
           <t>18/mai</t>
         </is>
@@ -1779,7 +1955,10 @@
       <c r="E59" t="n">
         <v>1</v>
       </c>
-      <c r="F59" t="inlineStr">
+      <c r="F59" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G59" t="inlineStr">
         <is>
           <t>19/mai</t>
         </is>
@@ -1803,7 +1982,10 @@
       <c r="E60" t="n">
         <v>0</v>
       </c>
-      <c r="F60" t="inlineStr">
+      <c r="F60" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G60" t="inlineStr">
         <is>
           <t>20/mai</t>
         </is>
@@ -1827,7 +2009,10 @@
       <c r="E61" t="n">
         <v>4</v>
       </c>
-      <c r="F61" t="inlineStr">
+      <c r="F61" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G61" t="inlineStr">
         <is>
           <t>21/mai</t>
         </is>
@@ -1851,7 +2036,10 @@
       <c r="E62" t="n">
         <v>0</v>
       </c>
-      <c r="F62" t="inlineStr">
+      <c r="F62" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G62" t="inlineStr">
         <is>
           <t>22/mai</t>
         </is>
@@ -1875,7 +2063,10 @@
       <c r="E63" t="n">
         <v>4</v>
       </c>
-      <c r="F63" t="inlineStr">
+      <c r="F63" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G63" t="inlineStr">
         <is>
           <t>23/mai</t>
         </is>
@@ -1899,7 +2090,10 @@
       <c r="E64" t="n">
         <v>1</v>
       </c>
-      <c r="F64" t="inlineStr">
+      <c r="F64" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G64" t="inlineStr">
         <is>
           <t>24/mai</t>
         </is>
@@ -1923,7 +2117,10 @@
       <c r="E65" t="n">
         <v>1</v>
       </c>
-      <c r="F65" t="inlineStr">
+      <c r="F65" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G65" t="inlineStr">
         <is>
           <t>25/mai</t>
         </is>
@@ -1947,7 +2144,10 @@
       <c r="E66" t="n">
         <v>1</v>
       </c>
-      <c r="F66" t="inlineStr">
+      <c r="F66" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G66" t="inlineStr">
         <is>
           <t>26/mai</t>
         </is>
@@ -1971,7 +2171,10 @@
       <c r="E67" t="n">
         <v>0</v>
       </c>
-      <c r="F67" t="inlineStr">
+      <c r="F67" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G67" t="inlineStr">
         <is>
           <t>27/mai</t>
         </is>
@@ -1995,7 +2198,10 @@
       <c r="E68" t="n">
         <v>3</v>
       </c>
-      <c r="F68" t="inlineStr">
+      <c r="F68" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G68" t="inlineStr">
         <is>
           <t>28/mai</t>
         </is>
@@ -2019,7 +2225,10 @@
       <c r="E69" t="n">
         <v>0</v>
       </c>
-      <c r="F69" t="inlineStr">
+      <c r="F69" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G69" t="inlineStr">
         <is>
           <t>29/mai</t>
         </is>
@@ -2043,7 +2252,10 @@
       <c r="E70" t="n">
         <v>3</v>
       </c>
-      <c r="F70" t="inlineStr">
+      <c r="F70" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G70" t="inlineStr">
         <is>
           <t>30/mai</t>
         </is>
@@ -2067,7 +2279,10 @@
       <c r="E71" t="n">
         <v>2</v>
       </c>
-      <c r="F71" t="inlineStr">
+      <c r="F71" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G71" t="inlineStr">
         <is>
           <t>31/mai</t>
         </is>
@@ -2091,7 +2306,10 @@
       <c r="E72" t="n">
         <v>3</v>
       </c>
-      <c r="F72" t="inlineStr">
+      <c r="F72" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G72" t="inlineStr">
         <is>
           <t>01/jun</t>
         </is>
@@ -2115,7 +2333,10 @@
       <c r="E73" t="n">
         <v>16</v>
       </c>
-      <c r="F73" t="inlineStr">
+      <c r="F73" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G73" t="inlineStr">
         <is>
           <t>02/jun</t>
         </is>
@@ -2139,7 +2360,10 @@
       <c r="E74" t="n">
         <v>3</v>
       </c>
-      <c r="F74" t="inlineStr">
+      <c r="F74" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G74" t="inlineStr">
         <is>
           <t>03/jun</t>
         </is>
@@ -2163,7 +2387,10 @@
       <c r="E75" t="n">
         <v>2</v>
       </c>
-      <c r="F75" t="inlineStr">
+      <c r="F75" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G75" t="inlineStr">
         <is>
           <t>04/jun</t>
         </is>
@@ -2187,7 +2414,10 @@
       <c r="E76" t="n">
         <v>31</v>
       </c>
-      <c r="F76" t="inlineStr">
+      <c r="F76" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G76" t="inlineStr">
         <is>
           <t>05/jun</t>
         </is>
@@ -2211,7 +2441,10 @@
       <c r="E77" t="n">
         <v>11</v>
       </c>
-      <c r="F77" t="inlineStr">
+      <c r="F77" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G77" t="inlineStr">
         <is>
           <t>06/jun</t>
         </is>
@@ -2235,7 +2468,10 @@
       <c r="E78" t="n">
         <v>19</v>
       </c>
-      <c r="F78" t="inlineStr">
+      <c r="F78" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G78" t="inlineStr">
         <is>
           <t>07/jun</t>
         </is>
@@ -2259,7 +2495,10 @@
       <c r="E79" t="n">
         <v>6</v>
       </c>
-      <c r="F79" t="inlineStr">
+      <c r="F79" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G79" t="inlineStr">
         <is>
           <t>08/jun</t>
         </is>
@@ -2283,7 +2522,10 @@
       <c r="E80" t="n">
         <v>3</v>
       </c>
-      <c r="F80" t="inlineStr">
+      <c r="F80" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G80" t="inlineStr">
         <is>
           <t>09/jun</t>
         </is>
@@ -2307,7 +2549,10 @@
       <c r="E81" t="n">
         <v>17</v>
       </c>
-      <c r="F81" t="inlineStr">
+      <c r="F81" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G81" t="inlineStr">
         <is>
           <t>10/jun</t>
         </is>
@@ -2331,7 +2576,10 @@
       <c r="E82" t="n">
         <v>15</v>
       </c>
-      <c r="F82" t="inlineStr">
+      <c r="F82" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G82" t="inlineStr">
         <is>
           <t>11/jun</t>
         </is>
@@ -2355,7 +2603,10 @@
       <c r="E83" t="n">
         <v>4</v>
       </c>
-      <c r="F83" t="inlineStr">
+      <c r="F83" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G83" t="inlineStr">
         <is>
           <t>12/jun</t>
         </is>
@@ -2379,7 +2630,10 @@
       <c r="E84" t="n">
         <v>0</v>
       </c>
-      <c r="F84" t="inlineStr">
+      <c r="F84" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G84" t="inlineStr">
         <is>
           <t>13/jun</t>
         </is>
@@ -2403,7 +2657,10 @@
       <c r="E85" t="n">
         <v>1</v>
       </c>
-      <c r="F85" t="inlineStr">
+      <c r="F85" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G85" t="inlineStr">
         <is>
           <t>14/jun</t>
         </is>
@@ -2427,7 +2684,10 @@
       <c r="E86" t="n">
         <v>4</v>
       </c>
-      <c r="F86" t="inlineStr">
+      <c r="F86" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G86" t="inlineStr">
         <is>
           <t>15/jun</t>
         </is>
@@ -2451,7 +2711,10 @@
       <c r="E87" t="n">
         <v>8</v>
       </c>
-      <c r="F87" t="inlineStr">
+      <c r="F87" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G87" t="inlineStr">
         <is>
           <t>16/jun</t>
         </is>
@@ -2475,7 +2738,10 @@
       <c r="E88" t="n">
         <v>20</v>
       </c>
-      <c r="F88" t="inlineStr">
+      <c r="F88" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G88" t="inlineStr">
         <is>
           <t>17/jun</t>
         </is>
@@ -2499,7 +2765,10 @@
       <c r="E89" t="n">
         <v>0</v>
       </c>
-      <c r="F89" t="inlineStr">
+      <c r="F89" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G89" t="inlineStr">
         <is>
           <t>18/jun</t>
         </is>
@@ -2523,7 +2792,10 @@
       <c r="E90" t="n">
         <v>3</v>
       </c>
-      <c r="F90" t="inlineStr">
+      <c r="F90" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G90" t="inlineStr">
         <is>
           <t>19/jun</t>
         </is>
@@ -2547,7 +2819,10 @@
       <c r="E91" t="n">
         <v>65</v>
       </c>
-      <c r="F91" t="inlineStr">
+      <c r="F91" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G91" t="inlineStr">
         <is>
           <t>20/jun</t>
         </is>
@@ -2571,7 +2846,10 @@
       <c r="E92" t="n">
         <v>48</v>
       </c>
-      <c r="F92" t="inlineStr">
+      <c r="F92" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G92" t="inlineStr">
         <is>
           <t>21/jun</t>
         </is>
@@ -2595,7 +2873,10 @@
       <c r="E93" t="n">
         <v>1</v>
       </c>
-      <c r="F93" t="inlineStr">
+      <c r="F93" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G93" t="inlineStr">
         <is>
           <t>22/jun</t>
         </is>
@@ -2619,7 +2900,10 @@
       <c r="E94" t="n">
         <v>21</v>
       </c>
-      <c r="F94" t="inlineStr">
+      <c r="F94" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G94" t="inlineStr">
         <is>
           <t>23/jun</t>
         </is>
@@ -2643,7 +2927,10 @@
       <c r="E95" t="n">
         <v>58</v>
       </c>
-      <c r="F95" t="inlineStr">
+      <c r="F95" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G95" t="inlineStr">
         <is>
           <t>24/jun</t>
         </is>
@@ -2667,7 +2954,10 @@
       <c r="E96" t="n">
         <v>37</v>
       </c>
-      <c r="F96" t="inlineStr">
+      <c r="F96" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G96" t="inlineStr">
         <is>
           <t>25/jun</t>
         </is>
@@ -2691,7 +2981,10 @@
       <c r="E97" t="n">
         <v>47</v>
       </c>
-      <c r="F97" t="inlineStr">
+      <c r="F97" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G97" t="inlineStr">
         <is>
           <t>26/jun</t>
         </is>
@@ -2715,7 +3008,10 @@
       <c r="E98" t="n">
         <v>76</v>
       </c>
-      <c r="F98" t="inlineStr">
+      <c r="F98" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G98" t="inlineStr">
         <is>
           <t>27/jun</t>
         </is>
@@ -2739,7 +3035,10 @@
       <c r="E99" t="n">
         <v>12</v>
       </c>
-      <c r="F99" t="inlineStr">
+      <c r="F99" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G99" t="inlineStr">
         <is>
           <t>28/jun</t>
         </is>
@@ -2763,7 +3062,10 @@
       <c r="E100" t="n">
         <v>21</v>
       </c>
-      <c r="F100" t="inlineStr">
+      <c r="F100" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G100" t="inlineStr">
         <is>
           <t>29/jun</t>
         </is>
@@ -2787,7 +3089,10 @@
       <c r="E101" t="n">
         <v>31</v>
       </c>
-      <c r="F101" t="inlineStr">
+      <c r="F101" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G101" t="inlineStr">
         <is>
           <t>30/jun</t>
         </is>
@@ -2811,7 +3116,10 @@
       <c r="E102" t="n">
         <v>100</v>
       </c>
-      <c r="F102" t="inlineStr">
+      <c r="F102" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G102" t="inlineStr">
         <is>
           <t>01/jul</t>
         </is>
@@ -2835,7 +3143,10 @@
       <c r="E103" t="n">
         <v>64</v>
       </c>
-      <c r="F103" t="inlineStr">
+      <c r="F103" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G103" t="inlineStr">
         <is>
           <t>02/jul</t>
         </is>
@@ -2859,7 +3170,10 @@
       <c r="E104" t="n">
         <v>81</v>
       </c>
-      <c r="F104" t="inlineStr">
+      <c r="F104" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G104" t="inlineStr">
         <is>
           <t>03/jul</t>
         </is>
@@ -2883,7 +3197,10 @@
       <c r="E105" t="n">
         <v>88</v>
       </c>
-      <c r="F105" t="inlineStr">
+      <c r="F105" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G105" t="inlineStr">
         <is>
           <t>04/jul</t>
         </is>
@@ -2907,7 +3224,10 @@
       <c r="E106" t="n">
         <v>62</v>
       </c>
-      <c r="F106" t="inlineStr">
+      <c r="F106" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G106" t="inlineStr">
         <is>
           <t>05/jul</t>
         </is>
@@ -2931,7 +3251,10 @@
       <c r="E107" t="n">
         <v>8</v>
       </c>
-      <c r="F107" t="inlineStr">
+      <c r="F107" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G107" t="inlineStr">
         <is>
           <t>06/jul</t>
         </is>
@@ -2955,7 +3278,10 @@
       <c r="E108" t="n">
         <v>25</v>
       </c>
-      <c r="F108" t="inlineStr">
+      <c r="F108" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G108" t="inlineStr">
         <is>
           <t>07/jul</t>
         </is>
@@ -2979,7 +3305,10 @@
       <c r="E109" t="n">
         <v>49</v>
       </c>
-      <c r="F109" t="inlineStr">
+      <c r="F109" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G109" t="inlineStr">
         <is>
           <t>08/jul</t>
         </is>
@@ -3003,7 +3332,10 @@
       <c r="E110" t="n">
         <v>97</v>
       </c>
-      <c r="F110" t="inlineStr">
+      <c r="F110" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G110" t="inlineStr">
         <is>
           <t>09/jul</t>
         </is>
@@ -3027,7 +3359,10 @@
       <c r="E111" t="n">
         <v>77</v>
       </c>
-      <c r="F111" t="inlineStr">
+      <c r="F111" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G111" t="inlineStr">
         <is>
           <t>10/jul</t>
         </is>
@@ -3051,7 +3386,10 @@
       <c r="E112" t="n">
         <v>89</v>
       </c>
-      <c r="F112" t="inlineStr">
+      <c r="F112" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G112" t="inlineStr">
         <is>
           <t>11/jul</t>
         </is>
@@ -3075,7 +3413,10 @@
       <c r="E113" t="n">
         <v>64</v>
       </c>
-      <c r="F113" t="inlineStr">
+      <c r="F113" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G113" t="inlineStr">
         <is>
           <t>12/jul</t>
         </is>
@@ -3099,7 +3440,10 @@
       <c r="E114" t="n">
         <v>6</v>
       </c>
-      <c r="F114" t="inlineStr">
+      <c r="F114" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G114" t="inlineStr">
         <is>
           <t>13/jul</t>
         </is>
@@ -3123,7 +3467,10 @@
       <c r="E115" t="n">
         <v>49</v>
       </c>
-      <c r="F115" t="inlineStr">
+      <c r="F115" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G115" t="inlineStr">
         <is>
           <t>14/jul</t>
         </is>
@@ -3147,7 +3494,10 @@
       <c r="E116" t="n">
         <v>43</v>
       </c>
-      <c r="F116" t="inlineStr">
+      <c r="F116" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G116" t="inlineStr">
         <is>
           <t>15/jul</t>
         </is>
@@ -3171,7 +3521,10 @@
       <c r="E117" t="n">
         <v>37</v>
       </c>
-      <c r="F117" t="inlineStr">
+      <c r="F117" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G117" t="inlineStr">
         <is>
           <t>16/jul</t>
         </is>
@@ -3195,7 +3548,10 @@
       <c r="E118" t="n">
         <v>33</v>
       </c>
-      <c r="F118" t="inlineStr">
+      <c r="F118" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G118" t="inlineStr">
         <is>
           <t>17/jul</t>
         </is>
@@ -3219,7 +3575,10 @@
       <c r="E119" t="n">
         <v>1</v>
       </c>
-      <c r="F119" t="inlineStr">
+      <c r="F119" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G119" t="inlineStr">
         <is>
           <t>18/jul</t>
         </is>
@@ -3243,7 +3602,10 @@
       <c r="E120" t="n">
         <v>64</v>
       </c>
-      <c r="F120" t="inlineStr">
+      <c r="F120" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G120" t="inlineStr">
         <is>
           <t>19/jul</t>
         </is>
@@ -3267,7 +3629,10 @@
       <c r="E121" t="n">
         <v>5</v>
       </c>
-      <c r="F121" t="inlineStr">
+      <c r="F121" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G121" t="inlineStr">
         <is>
           <t>20/jul</t>
         </is>
@@ -3291,7 +3656,10 @@
       <c r="E122" t="n">
         <v>33</v>
       </c>
-      <c r="F122" t="inlineStr">
+      <c r="F122" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G122" t="inlineStr">
         <is>
           <t>21/jul</t>
         </is>
@@ -3315,7 +3683,10 @@
       <c r="E123" t="n">
         <v>101</v>
       </c>
-      <c r="F123" t="inlineStr">
+      <c r="F123" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G123" t="inlineStr">
         <is>
           <t>22/jul</t>
         </is>
@@ -3339,7 +3710,10 @@
       <c r="E124" t="n">
         <v>151</v>
       </c>
-      <c r="F124" t="inlineStr">
+      <c r="F124" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G124" t="inlineStr">
         <is>
           <t>23/jul</t>
         </is>
@@ -3363,7 +3737,10 @@
       <c r="E125" t="n">
         <v>128</v>
       </c>
-      <c r="F125" t="inlineStr">
+      <c r="F125" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G125" t="inlineStr">
         <is>
           <t>24/jul</t>
         </is>
@@ -3387,7 +3764,10 @@
       <c r="E126" t="n">
         <v>170</v>
       </c>
-      <c r="F126" t="inlineStr">
+      <c r="F126" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G126" t="inlineStr">
         <is>
           <t>25/jul</t>
         </is>
@@ -3411,7 +3791,10 @@
       <c r="E127" t="n">
         <v>51</v>
       </c>
-      <c r="F127" t="inlineStr">
+      <c r="F127" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G127" t="inlineStr">
         <is>
           <t>26/jul</t>
         </is>
@@ -3435,7 +3818,10 @@
       <c r="E128" t="n">
         <v>2</v>
       </c>
-      <c r="F128" t="inlineStr">
+      <c r="F128" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G128" t="inlineStr">
         <is>
           <t>27/jul</t>
         </is>
@@ -3459,7 +3845,10 @@
       <c r="E129" t="n">
         <v>57</v>
       </c>
-      <c r="F129" t="inlineStr">
+      <c r="F129" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G129" t="inlineStr">
         <is>
           <t>28/jul</t>
         </is>
@@ -3483,7 +3872,10 @@
       <c r="E130" t="n">
         <v>99</v>
       </c>
-      <c r="F130" t="inlineStr">
+      <c r="F130" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G130" t="inlineStr">
         <is>
           <t>29/jul</t>
         </is>
@@ -3507,7 +3899,10 @@
       <c r="E131" t="n">
         <v>137</v>
       </c>
-      <c r="F131" t="inlineStr">
+      <c r="F131" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G131" t="inlineStr">
         <is>
           <t>30/jul</t>
         </is>
@@ -3531,7 +3926,10 @@
       <c r="E132" t="n">
         <v>166</v>
       </c>
-      <c r="F132" t="inlineStr">
+      <c r="F132" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G132" t="inlineStr">
         <is>
           <t>31/jul</t>
         </is>
@@ -3555,7 +3953,10 @@
       <c r="E133" t="n">
         <v>108</v>
       </c>
-      <c r="F133" t="inlineStr">
+      <c r="F133" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G133" t="inlineStr">
         <is>
           <t>01/ago</t>
         </is>
@@ -3579,7 +3980,10 @@
       <c r="E134" t="n">
         <v>39</v>
       </c>
-      <c r="F134" t="inlineStr">
+      <c r="F134" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G134" t="inlineStr">
         <is>
           <t>02/ago</t>
         </is>
@@ -3603,7 +4007,10 @@
       <c r="E135" t="n">
         <v>5</v>
       </c>
-      <c r="F135" t="inlineStr">
+      <c r="F135" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G135" t="inlineStr">
         <is>
           <t>03/ago</t>
         </is>
@@ -3627,7 +4034,10 @@
       <c r="E136" t="n">
         <v>64</v>
       </c>
-      <c r="F136" t="inlineStr">
+      <c r="F136" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G136" t="inlineStr">
         <is>
           <t>04/ago</t>
         </is>
@@ -3651,7 +4061,10 @@
       <c r="E137" t="n">
         <v>111</v>
       </c>
-      <c r="F137" t="inlineStr">
+      <c r="F137" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G137" t="inlineStr">
         <is>
           <t>05/ago</t>
         </is>
@@ -3675,7 +4088,10 @@
       <c r="E138" t="n">
         <v>77</v>
       </c>
-      <c r="F138" t="inlineStr">
+      <c r="F138" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G138" t="inlineStr">
         <is>
           <t>06/ago</t>
         </is>
@@ -3699,7 +4115,10 @@
       <c r="E139" t="n">
         <v>103</v>
       </c>
-      <c r="F139" t="inlineStr">
+      <c r="F139" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G139" t="inlineStr">
         <is>
           <t>07/ago</t>
         </is>
@@ -3723,7 +4142,10 @@
       <c r="E140" t="n">
         <v>135</v>
       </c>
-      <c r="F140" t="inlineStr">
+      <c r="F140" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G140" t="inlineStr">
         <is>
           <t>08/ago</t>
         </is>
@@ -3747,7 +4169,10 @@
       <c r="E141" t="n">
         <v>32</v>
       </c>
-      <c r="F141" t="inlineStr">
+      <c r="F141" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G141" t="inlineStr">
         <is>
           <t>09/ago</t>
         </is>
@@ -3771,7 +4196,10 @@
       <c r="E142" t="n">
         <v>3</v>
       </c>
-      <c r="F142" t="inlineStr">
+      <c r="F142" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G142" t="inlineStr">
         <is>
           <t>10/ago</t>
         </is>
@@ -3795,7 +4223,10 @@
       <c r="E143" t="n">
         <v>45</v>
       </c>
-      <c r="F143" t="inlineStr">
+      <c r="F143" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G143" t="inlineStr">
         <is>
           <t>11/ago</t>
         </is>
@@ -3819,7 +4250,10 @@
       <c r="E144" t="n">
         <v>105</v>
       </c>
-      <c r="F144" t="inlineStr">
+      <c r="F144" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G144" t="inlineStr">
         <is>
           <t>12/ago</t>
         </is>
@@ -3843,7 +4277,10 @@
       <c r="E145" t="n">
         <v>74</v>
       </c>
-      <c r="F145" t="inlineStr">
+      <c r="F145" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G145" t="inlineStr">
         <is>
           <t>13/ago</t>
         </is>
@@ -3867,7 +4304,10 @@
       <c r="E146" t="n">
         <v>65</v>
       </c>
-      <c r="F146" t="inlineStr">
+      <c r="F146" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G146" t="inlineStr">
         <is>
           <t>14/ago</t>
         </is>
@@ -3891,7 +4331,10 @@
       <c r="E147" t="n">
         <v>79</v>
       </c>
-      <c r="F147" t="inlineStr">
+      <c r="F147" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G147" t="inlineStr">
         <is>
           <t>15/ago</t>
         </is>
@@ -3915,7 +4358,10 @@
       <c r="E148" t="n">
         <v>27</v>
       </c>
-      <c r="F148" t="inlineStr">
+      <c r="F148" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G148" t="inlineStr">
         <is>
           <t>16/ago</t>
         </is>
@@ -3939,7 +4385,10 @@
       <c r="E149" t="n">
         <v>2</v>
       </c>
-      <c r="F149" t="inlineStr">
+      <c r="F149" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G149" t="inlineStr">
         <is>
           <t>17/ago</t>
         </is>
@@ -3963,7 +4412,10 @@
       <c r="E150" t="n">
         <v>54</v>
       </c>
-      <c r="F150" t="inlineStr">
+      <c r="F150" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G150" t="inlineStr">
         <is>
           <t>18/ago</t>
         </is>
@@ -3987,7 +4439,10 @@
       <c r="E151" t="n">
         <v>75</v>
       </c>
-      <c r="F151" t="inlineStr">
+      <c r="F151" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G151" t="inlineStr">
         <is>
           <t>19/ago</t>
         </is>
@@ -4011,7 +4466,10 @@
       <c r="E152" t="n">
         <v>61</v>
       </c>
-      <c r="F152" t="inlineStr">
+      <c r="F152" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G152" t="inlineStr">
         <is>
           <t>20/ago</t>
         </is>
@@ -4035,7 +4493,10 @@
       <c r="E153" t="n">
         <v>43</v>
       </c>
-      <c r="F153" t="inlineStr">
+      <c r="F153" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G153" t="inlineStr">
         <is>
           <t>21/ago</t>
         </is>
@@ -4059,7 +4520,10 @@
       <c r="E154" t="n">
         <v>45</v>
       </c>
-      <c r="F154" t="inlineStr">
+      <c r="F154" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G154" t="inlineStr">
         <is>
           <t>22/ago</t>
         </is>
@@ -4083,7 +4547,10 @@
       <c r="E155" t="n">
         <v>4</v>
       </c>
-      <c r="F155" t="inlineStr">
+      <c r="F155" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G155" t="inlineStr">
         <is>
           <t>23/ago</t>
         </is>
@@ -4107,7 +4574,10 @@
       <c r="E156" t="n">
         <v>1</v>
       </c>
-      <c r="F156" t="inlineStr">
+      <c r="F156" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G156" t="inlineStr">
         <is>
           <t>24/ago</t>
         </is>
@@ -4131,7 +4601,10 @@
       <c r="E157" t="n">
         <v>53</v>
       </c>
-      <c r="F157" t="inlineStr">
+      <c r="F157" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G157" t="inlineStr">
         <is>
           <t>25/ago</t>
         </is>
@@ -4155,7 +4628,10 @@
       <c r="E158" t="n">
         <v>66</v>
       </c>
-      <c r="F158" t="inlineStr">
+      <c r="F158" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G158" t="inlineStr">
         <is>
           <t>26/ago</t>
         </is>
@@ -4179,7 +4655,10 @@
       <c r="E159" t="n">
         <v>39</v>
       </c>
-      <c r="F159" t="inlineStr">
+      <c r="F159" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G159" t="inlineStr">
         <is>
           <t>27/ago</t>
         </is>
@@ -4203,7 +4682,10 @@
       <c r="E160" t="n">
         <v>36</v>
       </c>
-      <c r="F160" t="inlineStr">
+      <c r="F160" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G160" t="inlineStr">
         <is>
           <t>28/ago</t>
         </is>
@@ -4227,7 +4709,10 @@
       <c r="E161" t="n">
         <v>82</v>
       </c>
-      <c r="F161" t="inlineStr">
+      <c r="F161" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G161" t="inlineStr">
         <is>
           <t>29/ago</t>
         </is>
@@ -4251,7 +4736,10 @@
       <c r="E162" t="n">
         <v>9</v>
       </c>
-      <c r="F162" t="inlineStr">
+      <c r="F162" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G162" t="inlineStr">
         <is>
           <t>30/ago</t>
         </is>
@@ -4275,7 +4763,10 @@
       <c r="E163" t="n">
         <v>1</v>
       </c>
-      <c r="F163" t="inlineStr">
+      <c r="F163" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G163" t="inlineStr">
         <is>
           <t>31/ago</t>
         </is>
@@ -4299,7 +4790,10 @@
       <c r="E164" t="n">
         <v>34</v>
       </c>
-      <c r="F164" t="inlineStr">
+      <c r="F164" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G164" t="inlineStr">
         <is>
           <t>01/set</t>
         </is>
@@ -4323,7 +4817,10 @@
       <c r="E165" t="n">
         <v>85</v>
       </c>
-      <c r="F165" t="inlineStr">
+      <c r="F165" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G165" t="inlineStr">
         <is>
           <t>02/set</t>
         </is>
@@ -4347,7 +4844,10 @@
       <c r="E166" t="n">
         <v>53</v>
       </c>
-      <c r="F166" t="inlineStr">
+      <c r="F166" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G166" t="inlineStr">
         <is>
           <t>03/set</t>
         </is>
@@ -4371,7 +4871,10 @@
       <c r="E167" t="n">
         <v>35</v>
       </c>
-      <c r="F167" t="inlineStr">
+      <c r="F167" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G167" t="inlineStr">
         <is>
           <t>04/set</t>
         </is>
@@ -4395,7 +4898,10 @@
       <c r="E168" t="n">
         <v>30</v>
       </c>
-      <c r="F168" t="inlineStr">
+      <c r="F168" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G168" t="inlineStr">
         <is>
           <t>05/set</t>
         </is>
@@ -4419,7 +4925,10 @@
       <c r="E169" t="n">
         <v>14</v>
       </c>
-      <c r="F169" t="inlineStr">
+      <c r="F169" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G169" t="inlineStr">
         <is>
           <t>06/set</t>
         </is>
@@ -4443,7 +4952,10 @@
       <c r="E170" t="n">
         <v>1</v>
       </c>
-      <c r="F170" t="inlineStr">
+      <c r="F170" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G170" t="inlineStr">
         <is>
           <t>07/set</t>
         </is>
@@ -4467,7 +4979,10 @@
       <c r="E171" t="n">
         <v>1</v>
       </c>
-      <c r="F171" t="inlineStr">
+      <c r="F171" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G171" t="inlineStr">
         <is>
           <t>08/set</t>
         </is>
@@ -4491,7 +5006,10 @@
       <c r="E172" t="n">
         <v>0</v>
       </c>
-      <c r="F172" t="inlineStr">
+      <c r="F172" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G172" t="inlineStr">
         <is>
           <t>09/set</t>
         </is>
@@ -4515,7 +5033,10 @@
       <c r="E173" t="n">
         <v>26</v>
       </c>
-      <c r="F173" t="inlineStr">
+      <c r="F173" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G173" t="inlineStr">
         <is>
           <t>10/set</t>
         </is>
@@ -4539,7 +5060,10 @@
       <c r="E174" t="n">
         <v>36</v>
       </c>
-      <c r="F174" t="inlineStr">
+      <c r="F174" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G174" t="inlineStr">
         <is>
           <t>11/set</t>
         </is>
@@ -4563,7 +5087,10 @@
       <c r="E175" t="n">
         <v>56</v>
       </c>
-      <c r="F175" t="inlineStr">
+      <c r="F175" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G175" t="inlineStr">
         <is>
           <t>12/set</t>
         </is>
@@ -4587,7 +5114,10 @@
       <c r="E176" t="n">
         <v>15</v>
       </c>
-      <c r="F176" t="inlineStr">
+      <c r="F176" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G176" t="inlineStr">
         <is>
           <t>13/set</t>
         </is>
@@ -4611,7 +5141,10 @@
       <c r="E177" t="n">
         <v>4</v>
       </c>
-      <c r="F177" t="inlineStr">
+      <c r="F177" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G177" t="inlineStr">
         <is>
           <t>14/set</t>
         </is>
@@ -4635,7 +5168,10 @@
       <c r="E178" t="n">
         <v>10</v>
       </c>
-      <c r="F178" t="inlineStr">
+      <c r="F178" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G178" t="inlineStr">
         <is>
           <t>15/set</t>
         </is>
@@ -4659,7 +5195,10 @@
       <c r="E179" t="n">
         <v>60</v>
       </c>
-      <c r="F179" t="inlineStr">
+      <c r="F179" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G179" t="inlineStr">
         <is>
           <t>16/set</t>
         </is>
@@ -4683,7 +5222,10 @@
       <c r="E180" t="n">
         <v>33</v>
       </c>
-      <c r="F180" t="inlineStr">
+      <c r="F180" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G180" t="inlineStr">
         <is>
           <t>17/set</t>
         </is>
@@ -4707,7 +5249,10 @@
       <c r="E181" t="n">
         <v>25</v>
       </c>
-      <c r="F181" t="inlineStr">
+      <c r="F181" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G181" t="inlineStr">
         <is>
           <t>18/set</t>
         </is>
@@ -4731,7 +5276,10 @@
       <c r="E182" t="n">
         <v>29</v>
       </c>
-      <c r="F182" t="inlineStr">
+      <c r="F182" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G182" t="inlineStr">
         <is>
           <t>19/set</t>
         </is>
@@ -4755,7 +5303,10 @@
       <c r="E183" t="n">
         <v>14</v>
       </c>
-      <c r="F183" t="inlineStr">
+      <c r="F183" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G183" t="inlineStr">
         <is>
           <t>20/set</t>
         </is>
@@ -4779,7 +5330,10 @@
       <c r="E184" t="n">
         <v>0</v>
       </c>
-      <c r="F184" t="inlineStr">
+      <c r="F184" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G184" t="inlineStr">
         <is>
           <t>21/set</t>
         </is>
@@ -4803,7 +5357,10 @@
       <c r="E185" t="n">
         <v>7</v>
       </c>
-      <c r="F185" t="inlineStr">
+      <c r="F185" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G185" t="inlineStr">
         <is>
           <t>22/set</t>
         </is>
@@ -4827,7 +5384,10 @@
       <c r="E186" t="n">
         <v>30</v>
       </c>
-      <c r="F186" t="inlineStr">
+      <c r="F186" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G186" t="inlineStr">
         <is>
           <t>23/set</t>
         </is>
@@ -4851,7 +5411,10 @@
       <c r="E187" t="n">
         <v>27</v>
       </c>
-      <c r="F187" t="inlineStr">
+      <c r="F187" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G187" t="inlineStr">
         <is>
           <t>24/set</t>
         </is>
@@ -4875,7 +5438,10 @@
       <c r="E188" t="n">
         <v>27</v>
       </c>
-      <c r="F188" t="inlineStr">
+      <c r="F188" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G188" t="inlineStr">
         <is>
           <t>25/set</t>
         </is>
@@ -4899,7 +5465,10 @@
       <c r="E189" t="n">
         <v>28</v>
       </c>
-      <c r="F189" t="inlineStr">
+      <c r="F189" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G189" t="inlineStr">
         <is>
           <t>26/set</t>
         </is>
@@ -4923,7 +5492,10 @@
       <c r="E190" t="n">
         <v>8</v>
       </c>
-      <c r="F190" t="inlineStr">
+      <c r="F190" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G190" t="inlineStr">
         <is>
           <t>27/set</t>
         </is>
@@ -4947,7 +5519,10 @@
       <c r="E191" t="n">
         <v>0</v>
       </c>
-      <c r="F191" t="inlineStr">
+      <c r="F191" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G191" t="inlineStr">
         <is>
           <t>28/set</t>
         </is>
@@ -4971,7 +5546,10 @@
       <c r="E192" t="n">
         <v>13</v>
       </c>
-      <c r="F192" t="inlineStr">
+      <c r="F192" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G192" t="inlineStr">
         <is>
           <t>29/set</t>
         </is>
@@ -4995,7 +5573,10 @@
       <c r="E193" t="n">
         <v>31</v>
       </c>
-      <c r="F193" t="inlineStr">
+      <c r="F193" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G193" t="inlineStr">
         <is>
           <t>30/set</t>
         </is>
@@ -5019,7 +5600,10 @@
       <c r="E194" t="n">
         <v>36</v>
       </c>
-      <c r="F194" t="inlineStr">
+      <c r="F194" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G194" t="inlineStr">
         <is>
           <t>01/out</t>
         </is>
@@ -5043,7 +5627,10 @@
       <c r="E195" t="n">
         <v>17</v>
       </c>
-      <c r="F195" t="inlineStr">
+      <c r="F195" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G195" t="inlineStr">
         <is>
           <t>02/out</t>
         </is>
@@ -5067,7 +5654,10 @@
       <c r="E196" t="n">
         <v>27</v>
       </c>
-      <c r="F196" t="inlineStr">
+      <c r="F196" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G196" t="inlineStr">
         <is>
           <t>03/out</t>
         </is>
@@ -5091,7 +5681,10 @@
       <c r="E197" t="n">
         <v>13</v>
       </c>
-      <c r="F197" t="inlineStr">
+      <c r="F197" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G197" t="inlineStr">
         <is>
           <t>04/out</t>
         </is>
@@ -5115,7 +5708,10 @@
       <c r="E198" t="n">
         <v>0</v>
       </c>
-      <c r="F198" t="inlineStr">
+      <c r="F198" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G198" t="inlineStr">
         <is>
           <t>05/out</t>
         </is>
@@ -5139,7 +5735,10 @@
       <c r="E199" t="n">
         <v>11</v>
       </c>
-      <c r="F199" t="inlineStr">
+      <c r="F199" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G199" t="inlineStr">
         <is>
           <t>06/out</t>
         </is>
@@ -5163,7 +5762,10 @@
       <c r="E200" t="n">
         <v>15</v>
       </c>
-      <c r="F200" t="inlineStr">
+      <c r="F200" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G200" t="inlineStr">
         <is>
           <t>07/out</t>
         </is>
@@ -5187,7 +5789,10 @@
       <c r="E201" t="n">
         <v>33</v>
       </c>
-      <c r="F201" t="inlineStr">
+      <c r="F201" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G201" t="inlineStr">
         <is>
           <t>08/out</t>
         </is>
@@ -5211,7 +5816,10 @@
       <c r="E202" t="n">
         <v>18</v>
       </c>
-      <c r="F202" t="inlineStr">
+      <c r="F202" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G202" t="inlineStr">
         <is>
           <t>09/out</t>
         </is>
@@ -5235,7 +5843,10 @@
       <c r="E203" t="n">
         <v>22</v>
       </c>
-      <c r="F203" t="inlineStr">
+      <c r="F203" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G203" t="inlineStr">
         <is>
           <t>10/out</t>
         </is>
@@ -5259,7 +5870,10 @@
       <c r="E204" t="n">
         <v>24</v>
       </c>
-      <c r="F204" t="inlineStr">
+      <c r="F204" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G204" t="inlineStr">
         <is>
           <t>11/out</t>
         </is>
@@ -5283,7 +5897,10 @@
       <c r="E205" t="n">
         <v>0</v>
       </c>
-      <c r="F205" t="inlineStr">
+      <c r="F205" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G205" t="inlineStr">
         <is>
           <t>12/out</t>
         </is>
@@ -5307,7 +5924,10 @@
       <c r="E206" t="n">
         <v>1</v>
       </c>
-      <c r="F206" t="inlineStr">
+      <c r="F206" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G206" t="inlineStr">
         <is>
           <t>13/out</t>
         </is>
@@ -5331,7 +5951,10 @@
       <c r="E207" t="n">
         <v>19</v>
       </c>
-      <c r="F207" t="inlineStr">
+      <c r="F207" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G207" t="inlineStr">
         <is>
           <t>14/out</t>
         </is>
@@ -5355,7 +5978,10 @@
       <c r="E208" t="n">
         <v>56</v>
       </c>
-      <c r="F208" t="inlineStr">
+      <c r="F208" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G208" t="inlineStr">
         <is>
           <t>15/out</t>
         </is>
@@ -5379,7 +6005,10 @@
       <c r="E209" t="n">
         <v>32</v>
       </c>
-      <c r="F209" t="inlineStr">
+      <c r="F209" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G209" t="inlineStr">
         <is>
           <t>16/out</t>
         </is>
@@ -5403,7 +6032,10 @@
       <c r="E210" t="n">
         <v>34</v>
       </c>
-      <c r="F210" t="inlineStr">
+      <c r="F210" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G210" t="inlineStr">
         <is>
           <t>17/out</t>
         </is>
@@ -5427,7 +6059,10 @@
       <c r="E211" t="n">
         <v>35</v>
       </c>
-      <c r="F211" t="inlineStr">
+      <c r="F211" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G211" t="inlineStr">
         <is>
           <t>18/out</t>
         </is>
@@ -5451,7 +6086,10 @@
       <c r="E212" t="n">
         <v>9</v>
       </c>
-      <c r="F212" t="inlineStr">
+      <c r="F212" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G212" t="inlineStr">
         <is>
           <t>19/out</t>
         </is>
@@ -5475,7 +6113,10 @@
       <c r="E213" t="n">
         <v>18</v>
       </c>
-      <c r="F213" t="inlineStr">
+      <c r="F213" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G213" t="inlineStr">
         <is>
           <t>20/out</t>
         </is>
@@ -5499,7 +6140,10 @@
       <c r="E214" t="n">
         <v>35</v>
       </c>
-      <c r="F214" t="inlineStr">
+      <c r="F214" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G214" t="inlineStr">
         <is>
           <t>21/out</t>
         </is>
@@ -5523,7 +6167,10 @@
       <c r="E215" t="n">
         <v>29</v>
       </c>
-      <c r="F215" t="inlineStr">
+      <c r="F215" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G215" t="inlineStr">
         <is>
           <t>22/out</t>
         </is>
@@ -5547,7 +6194,10 @@
       <c r="E216" t="n">
         <v>44</v>
       </c>
-      <c r="F216" t="inlineStr">
+      <c r="F216" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G216" t="inlineStr">
         <is>
           <t>23/out</t>
         </is>
@@ -5571,7 +6221,10 @@
       <c r="E217" t="n">
         <v>45</v>
       </c>
-      <c r="F217" t="inlineStr">
+      <c r="F217" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G217" t="inlineStr">
         <is>
           <t>24/out</t>
         </is>
@@ -5595,7 +6248,10 @@
       <c r="E218" t="n">
         <v>35</v>
       </c>
-      <c r="F218" t="inlineStr">
+      <c r="F218" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G218" t="inlineStr">
         <is>
           <t>25/out</t>
         </is>
@@ -5619,7 +6275,10 @@
       <c r="E219" t="n">
         <v>10</v>
       </c>
-      <c r="F219" t="inlineStr">
+      <c r="F219" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G219" t="inlineStr">
         <is>
           <t>26/out</t>
         </is>
@@ -5643,7 +6302,10 @@
       <c r="E220" t="n">
         <v>12</v>
       </c>
-      <c r="F220" t="inlineStr">
+      <c r="F220" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G220" t="inlineStr">
         <is>
           <t>27/out</t>
         </is>
@@ -5667,7 +6329,10 @@
       <c r="E221" t="n">
         <v>56</v>
       </c>
-      <c r="F221" t="inlineStr">
+      <c r="F221" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G221" t="inlineStr">
         <is>
           <t>28/out</t>
         </is>
@@ -5691,7 +6356,10 @@
       <c r="E222" t="n">
         <v>75</v>
       </c>
-      <c r="F222" t="inlineStr">
+      <c r="F222" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G222" t="inlineStr">
         <is>
           <t>29/out</t>
         </is>
@@ -5715,7 +6383,10 @@
       <c r="E223" t="n">
         <v>72</v>
       </c>
-      <c r="F223" t="inlineStr">
+      <c r="F223" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G223" t="inlineStr">
         <is>
           <t>30/out</t>
         </is>
@@ -5739,7 +6410,10 @@
       <c r="E224" t="n">
         <v>38</v>
       </c>
-      <c r="F224" t="inlineStr">
+      <c r="F224" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G224" t="inlineStr">
         <is>
           <t>31/out</t>
         </is>
@@ -5763,7 +6437,10 @@
       <c r="E225" t="n">
         <v>0</v>
       </c>
-      <c r="F225" t="inlineStr">
+      <c r="F225" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G225" t="inlineStr">
         <is>
           <t>01/nov</t>
         </is>
@@ -5787,7 +6464,10 @@
       <c r="E226" t="n">
         <v>2</v>
       </c>
-      <c r="F226" t="inlineStr">
+      <c r="F226" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G226" t="inlineStr">
         <is>
           <t>02/nov</t>
         </is>
@@ -5811,7 +6491,10 @@
       <c r="E227" t="n">
         <v>1</v>
       </c>
-      <c r="F227" t="inlineStr">
+      <c r="F227" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G227" t="inlineStr">
         <is>
           <t>03/nov</t>
         </is>
@@ -5835,7 +6518,10 @@
       <c r="E228" t="n">
         <v>2</v>
       </c>
-      <c r="F228" t="inlineStr">
+      <c r="F228" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G228" t="inlineStr">
         <is>
           <t>04/nov</t>
         </is>
@@ -5859,7 +6545,10 @@
       <c r="E229" t="n">
         <v>39</v>
       </c>
-      <c r="F229" t="inlineStr">
+      <c r="F229" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G229" t="inlineStr">
         <is>
           <t>05/nov</t>
         </is>
@@ -5883,7 +6572,10 @@
       <c r="E230" t="n">
         <v>64</v>
       </c>
-      <c r="F230" t="inlineStr">
+      <c r="F230" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G230" t="inlineStr">
         <is>
           <t>06/nov</t>
         </is>
@@ -5907,7 +6599,10 @@
       <c r="E231" t="n">
         <v>66</v>
       </c>
-      <c r="F231" t="inlineStr">
+      <c r="F231" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G231" t="inlineStr">
         <is>
           <t>07/nov</t>
         </is>
@@ -5931,7 +6626,10 @@
       <c r="E232" t="n">
         <v>51</v>
       </c>
-      <c r="F232" t="inlineStr">
+      <c r="F232" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G232" t="inlineStr">
         <is>
           <t>08/nov</t>
         </is>
@@ -5955,7 +6653,10 @@
       <c r="E233" t="n">
         <v>0</v>
       </c>
-      <c r="F233" t="inlineStr">
+      <c r="F233" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G233" t="inlineStr">
         <is>
           <t>09/nov</t>
         </is>
@@ -5979,7 +6680,10 @@
       <c r="E234" t="n">
         <v>31</v>
       </c>
-      <c r="F234" t="inlineStr">
+      <c r="F234" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G234" t="inlineStr">
         <is>
           <t>10/nov</t>
         </is>
@@ -6003,7 +6707,10 @@
       <c r="E235" t="n">
         <v>74</v>
       </c>
-      <c r="F235" t="inlineStr">
+      <c r="F235" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G235" t="inlineStr">
         <is>
           <t>11/nov</t>
         </is>
@@ -6027,7 +6734,10 @@
       <c r="E236" t="n">
         <v>87</v>
       </c>
-      <c r="F236" t="inlineStr">
+      <c r="F236" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G236" t="inlineStr">
         <is>
           <t>12/nov</t>
         </is>
@@ -6051,7 +6761,10 @@
       <c r="E237" t="n">
         <v>69</v>
       </c>
-      <c r="F237" t="inlineStr">
+      <c r="F237" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G237" t="inlineStr">
         <is>
           <t>13/nov</t>
         </is>
@@ -6075,7 +6788,10 @@
       <c r="E238" t="n">
         <v>69</v>
       </c>
-      <c r="F238" t="inlineStr">
+      <c r="F238" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G238" t="inlineStr">
         <is>
           <t>14/nov</t>
         </is>
@@ -6099,7 +6815,10 @@
       <c r="E239" t="n">
         <v>36</v>
       </c>
-      <c r="F239" t="inlineStr">
+      <c r="F239" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G239" t="inlineStr">
         <is>
           <t>15/nov</t>
         </is>
@@ -6123,7 +6842,10 @@
       <c r="E240" t="n">
         <v>0</v>
       </c>
-      <c r="F240" t="inlineStr">
+      <c r="F240" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G240" t="inlineStr">
         <is>
           <t>16/nov</t>
         </is>
@@ -6147,7 +6869,10 @@
       <c r="E241" t="n">
         <v>1</v>
       </c>
-      <c r="F241" t="inlineStr">
+      <c r="F241" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G241" t="inlineStr">
         <is>
           <t>17/nov</t>
         </is>
@@ -6171,7 +6896,10 @@
       <c r="E242" t="n">
         <v>24</v>
       </c>
-      <c r="F242" t="inlineStr">
+      <c r="F242" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G242" t="inlineStr">
         <is>
           <t>18/nov</t>
         </is>
@@ -6195,7 +6923,10 @@
       <c r="E243" t="n">
         <v>96</v>
       </c>
-      <c r="F243" t="inlineStr">
+      <c r="F243" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G243" t="inlineStr">
         <is>
           <t>19/nov</t>
         </is>
@@ -6219,7 +6950,10 @@
       <c r="E244" t="n">
         <v>56</v>
       </c>
-      <c r="F244" t="inlineStr">
+      <c r="F244" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G244" t="inlineStr">
         <is>
           <t>20/nov</t>
         </is>
@@ -6243,7 +6977,10 @@
       <c r="E245" t="n">
         <v>22</v>
       </c>
-      <c r="F245" t="inlineStr">
+      <c r="F245" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G245" t="inlineStr">
         <is>
           <t>21/nov</t>
         </is>
@@ -6267,7 +7004,10 @@
       <c r="E246" t="n">
         <v>25</v>
       </c>
-      <c r="F246" t="inlineStr">
+      <c r="F246" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G246" t="inlineStr">
         <is>
           <t>22/nov</t>
         </is>
@@ -6291,7 +7031,10 @@
       <c r="E247" t="n">
         <v>2</v>
       </c>
-      <c r="F247" t="inlineStr">
+      <c r="F247" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G247" t="inlineStr">
         <is>
           <t>23/nov</t>
         </is>
@@ -6315,7 +7058,10 @@
       <c r="E248" t="n">
         <v>4</v>
       </c>
-      <c r="F248" t="inlineStr">
+      <c r="F248" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G248" t="inlineStr">
         <is>
           <t>24/nov</t>
         </is>
@@ -6339,7 +7085,10 @@
       <c r="E249" t="n">
         <v>34</v>
       </c>
-      <c r="F249" t="inlineStr">
+      <c r="F249" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G249" t="inlineStr">
         <is>
           <t>25/nov</t>
         </is>
@@ -6363,7 +7112,10 @@
       <c r="E250" t="n">
         <v>40</v>
       </c>
-      <c r="F250" t="inlineStr">
+      <c r="F250" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G250" t="inlineStr">
         <is>
           <t>26/nov</t>
         </is>
@@ -6387,7 +7139,10 @@
       <c r="E251" t="n">
         <v>14</v>
       </c>
-      <c r="F251" t="inlineStr">
+      <c r="F251" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G251" t="inlineStr">
         <is>
           <t>27/nov</t>
         </is>
@@ -6411,7 +7166,10 @@
       <c r="E252" t="n">
         <v>52</v>
       </c>
-      <c r="F252" t="inlineStr">
+      <c r="F252" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G252" t="inlineStr">
         <is>
           <t>28/nov</t>
         </is>
@@ -6435,7 +7193,10 @@
       <c r="E253" t="n">
         <v>72</v>
       </c>
-      <c r="F253" t="inlineStr">
+      <c r="F253" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G253" t="inlineStr">
         <is>
           <t>29/nov</t>
         </is>
@@ -6459,7 +7220,10 @@
       <c r="E254" t="n">
         <v>12</v>
       </c>
-      <c r="F254" t="inlineStr">
+      <c r="F254" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G254" t="inlineStr">
         <is>
           <t>30/nov</t>
         </is>
@@ -6483,7 +7247,10 @@
       <c r="E255" t="n">
         <v>21</v>
       </c>
-      <c r="F255" t="inlineStr">
+      <c r="F255" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G255" t="inlineStr">
         <is>
           <t>01/dez</t>
         </is>
@@ -6507,7 +7274,10 @@
       <c r="E256" t="n">
         <v>31</v>
       </c>
-      <c r="F256" t="inlineStr">
+      <c r="F256" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G256" t="inlineStr">
         <is>
           <t>02/dez</t>
         </is>
@@ -6531,7 +7301,10 @@
       <c r="E257" t="n">
         <v>89</v>
       </c>
-      <c r="F257" t="inlineStr">
+      <c r="F257" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G257" t="inlineStr">
         <is>
           <t>03/dez</t>
         </is>
@@ -6555,7 +7328,10 @@
       <c r="E258" t="n">
         <v>35</v>
       </c>
-      <c r="F258" t="inlineStr">
+      <c r="F258" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G258" t="inlineStr">
         <is>
           <t>04/dez</t>
         </is>
@@ -6579,7 +7355,10 @@
       <c r="E259" t="n">
         <v>36</v>
       </c>
-      <c r="F259" t="inlineStr">
+      <c r="F259" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G259" t="inlineStr">
         <is>
           <t>05/dez</t>
         </is>
@@ -6603,7 +7382,10 @@
       <c r="E260" t="n">
         <v>45</v>
       </c>
-      <c r="F260" t="inlineStr">
+      <c r="F260" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G260" t="inlineStr">
         <is>
           <t>06/dez</t>
         </is>
@@ -6627,7 +7409,10 @@
       <c r="E261" t="n">
         <v>0</v>
       </c>
-      <c r="F261" t="inlineStr">
+      <c r="F261" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G261" t="inlineStr">
         <is>
           <t>07/dez</t>
         </is>
@@ -6651,7 +7436,10 @@
       <c r="E262" t="n">
         <v>7</v>
       </c>
-      <c r="F262" t="inlineStr">
+      <c r="F262" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G262" t="inlineStr">
         <is>
           <t>08/dez</t>
         </is>
@@ -6675,7 +7463,10 @@
       <c r="E263" t="n">
         <v>24</v>
       </c>
-      <c r="F263" t="inlineStr">
+      <c r="F263" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G263" t="inlineStr">
         <is>
           <t>09/dez</t>
         </is>
@@ -6699,7 +7490,10 @@
       <c r="E264" t="n">
         <v>43</v>
       </c>
-      <c r="F264" t="inlineStr">
+      <c r="F264" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G264" t="inlineStr">
         <is>
           <t>10/dez</t>
         </is>
@@ -6723,7 +7517,10 @@
       <c r="E265" t="n">
         <v>44</v>
       </c>
-      <c r="F265" t="inlineStr">
+      <c r="F265" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G265" t="inlineStr">
         <is>
           <t>11/dez</t>
         </is>
@@ -6747,7 +7544,10 @@
       <c r="E266" t="n">
         <v>48</v>
       </c>
-      <c r="F266" t="inlineStr">
+      <c r="F266" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G266" t="inlineStr">
         <is>
           <t>12/dez</t>
         </is>
@@ -6771,7 +7571,10 @@
       <c r="E267" t="n">
         <v>30</v>
       </c>
-      <c r="F267" t="inlineStr">
+      <c r="F267" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G267" t="inlineStr">
         <is>
           <t>13/dez</t>
         </is>
@@ -6795,7 +7598,10 @@
       <c r="E268" t="n">
         <v>9</v>
       </c>
-      <c r="F268" t="inlineStr">
+      <c r="F268" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G268" t="inlineStr">
         <is>
           <t>14/dez</t>
         </is>
@@ -6819,7 +7625,10 @@
       <c r="E269" t="n">
         <v>5</v>
       </c>
-      <c r="F269" t="inlineStr">
+      <c r="F269" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G269" t="inlineStr">
         <is>
           <t>15/dez</t>
         </is>
@@ -6843,7 +7652,10 @@
       <c r="E270" t="n">
         <v>35</v>
       </c>
-      <c r="F270" t="inlineStr">
+      <c r="F270" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G270" t="inlineStr">
         <is>
           <t>16/dez</t>
         </is>
@@ -6867,7 +7679,10 @@
       <c r="E271" t="n">
         <v>41</v>
       </c>
-      <c r="F271" t="inlineStr">
+      <c r="F271" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G271" t="inlineStr">
         <is>
           <t>17/dez</t>
         </is>
@@ -6891,7 +7706,10 @@
       <c r="E272" t="n">
         <v>47</v>
       </c>
-      <c r="F272" t="inlineStr">
+      <c r="F272" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G272" t="inlineStr">
         <is>
           <t>18/dez</t>
         </is>
@@ -6915,7 +7733,10 @@
       <c r="E273" t="n">
         <v>38</v>
       </c>
-      <c r="F273" t="inlineStr">
+      <c r="F273" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G273" t="inlineStr">
         <is>
           <t>19/dez</t>
         </is>
@@ -6939,7 +7760,10 @@
       <c r="E274" t="n">
         <v>46</v>
       </c>
-      <c r="F274" t="inlineStr">
+      <c r="F274" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G274" t="inlineStr">
         <is>
           <t>20/dez</t>
         </is>
@@ -6963,7 +7787,10 @@
       <c r="E275" t="n">
         <v>6</v>
       </c>
-      <c r="F275" t="inlineStr">
+      <c r="F275" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G275" t="inlineStr">
         <is>
           <t>21/dez</t>
         </is>
@@ -6987,7 +7814,10 @@
       <c r="E276" t="n">
         <v>13</v>
       </c>
-      <c r="F276" t="inlineStr">
+      <c r="F276" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G276" t="inlineStr">
         <is>
           <t>22/dez</t>
         </is>
@@ -7011,7 +7841,10 @@
       <c r="E277" t="n">
         <v>18</v>
       </c>
-      <c r="F277" t="inlineStr">
+      <c r="F277" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G277" t="inlineStr">
         <is>
           <t>23/dez</t>
         </is>
@@ -7035,7 +7868,10 @@
       <c r="E278" t="n">
         <v>40</v>
       </c>
-      <c r="F278" t="inlineStr">
+      <c r="F278" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G278" t="inlineStr">
         <is>
           <t>24/dez</t>
         </is>
@@ -7059,7 +7895,10 @@
       <c r="E279" t="n">
         <v>21</v>
       </c>
-      <c r="F279" t="inlineStr">
+      <c r="F279" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G279" t="inlineStr">
         <is>
           <t>25/dez</t>
         </is>
@@ -7083,7 +7922,10 @@
       <c r="E280" t="n">
         <v>16</v>
       </c>
-      <c r="F280" t="inlineStr">
+      <c r="F280" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G280" t="inlineStr">
         <is>
           <t>26/dez</t>
         </is>
@@ -7107,7 +7949,10 @@
       <c r="E281" t="n">
         <v>3</v>
       </c>
-      <c r="F281" t="inlineStr">
+      <c r="F281" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G281" t="inlineStr">
         <is>
           <t>27/dez</t>
         </is>
@@ -7131,7 +7976,10 @@
       <c r="E282" t="n">
         <v>6</v>
       </c>
-      <c r="F282" t="inlineStr">
+      <c r="F282" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G282" t="inlineStr">
         <is>
           <t>28/dez</t>
         </is>
@@ -7155,7 +8003,10 @@
       <c r="E283" t="n">
         <v>10</v>
       </c>
-      <c r="F283" t="inlineStr">
+      <c r="F283" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G283" t="inlineStr">
         <is>
           <t>29/dez</t>
         </is>
@@ -7179,7 +8030,10 @@
       <c r="E284" t="n">
         <v>21</v>
       </c>
-      <c r="F284" t="inlineStr">
+      <c r="F284" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G284" t="inlineStr">
         <is>
           <t>30/dez</t>
         </is>
@@ -7203,7 +8057,10 @@
       <c r="E285" t="n">
         <v>24</v>
       </c>
-      <c r="F285" t="inlineStr">
+      <c r="F285" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G285" t="inlineStr">
         <is>
           <t>31/dez</t>
         </is>
@@ -7227,7 +8084,10 @@
       <c r="E286" t="n">
         <v>18</v>
       </c>
-      <c r="F286" t="inlineStr">
+      <c r="F286" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G286" t="inlineStr">
         <is>
           <t>01/jan</t>
         </is>
@@ -7251,7 +8111,10 @@
       <c r="E287" t="n">
         <v>4</v>
       </c>
-      <c r="F287" t="inlineStr">
+      <c r="F287" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G287" t="inlineStr">
         <is>
           <t>02/jan</t>
         </is>
@@ -7275,7 +8138,10 @@
       <c r="E288" t="n">
         <v>3</v>
       </c>
-      <c r="F288" t="inlineStr">
+      <c r="F288" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G288" t="inlineStr">
         <is>
           <t>03/jan</t>
         </is>
@@ -7299,7 +8165,10 @@
       <c r="E289" t="n">
         <v>16</v>
       </c>
-      <c r="F289" t="inlineStr">
+      <c r="F289" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G289" t="inlineStr">
         <is>
           <t>04/jan</t>
         </is>
@@ -7323,7 +8192,10 @@
       <c r="E290" t="n">
         <v>11</v>
       </c>
-      <c r="F290" t="inlineStr">
+      <c r="F290" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G290" t="inlineStr">
         <is>
           <t>05/jan</t>
         </is>
@@ -7347,7 +8219,10 @@
       <c r="E291" t="n">
         <v>32</v>
       </c>
-      <c r="F291" t="inlineStr">
+      <c r="F291" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G291" t="inlineStr">
         <is>
           <t>06/jan</t>
         </is>
@@ -7371,7 +8246,10 @@
       <c r="E292" t="n">
         <v>33</v>
       </c>
-      <c r="F292" t="inlineStr">
+      <c r="F292" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G292" t="inlineStr">
         <is>
           <t>07/jan</t>
         </is>
@@ -7395,7 +8273,10 @@
       <c r="E293" t="n">
         <v>27</v>
       </c>
-      <c r="F293" t="inlineStr">
+      <c r="F293" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G293" t="inlineStr">
         <is>
           <t>08/jan</t>
         </is>
@@ -7419,7 +8300,10 @@
       <c r="E294" t="n">
         <v>32</v>
       </c>
-      <c r="F294" t="inlineStr">
+      <c r="F294" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G294" t="inlineStr">
         <is>
           <t>09/jan</t>
         </is>
@@ -7443,7 +8327,10 @@
       <c r="E295" t="n">
         <v>9</v>
       </c>
-      <c r="F295" t="inlineStr">
+      <c r="F295" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G295" t="inlineStr">
         <is>
           <t>10/jan</t>
         </is>
@@ -7467,7 +8354,10 @@
       <c r="E296" t="n">
         <v>31</v>
       </c>
-      <c r="F296" t="inlineStr">
+      <c r="F296" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G296" t="inlineStr">
         <is>
           <t>11/jan</t>
         </is>
@@ -7491,7 +8381,10 @@
       <c r="E297" t="n">
         <v>16</v>
       </c>
-      <c r="F297" t="inlineStr">
+      <c r="F297" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G297" t="inlineStr">
         <is>
           <t>12/jan</t>
         </is>
@@ -7515,7 +8408,10 @@
       <c r="E298" t="n">
         <v>49</v>
       </c>
-      <c r="F298" t="inlineStr">
+      <c r="F298" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G298" t="inlineStr">
         <is>
           <t>13/jan</t>
         </is>
@@ -7539,7 +8435,10 @@
       <c r="E299" t="n">
         <v>18</v>
       </c>
-      <c r="F299" t="inlineStr">
+      <c r="F299" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G299" t="inlineStr">
         <is>
           <t>14/jan</t>
         </is>
@@ -7563,7 +8462,10 @@
       <c r="E300" t="n">
         <v>22</v>
       </c>
-      <c r="F300" t="inlineStr">
+      <c r="F300" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G300" t="inlineStr">
         <is>
           <t>15/jan</t>
         </is>
@@ -7587,7 +8489,10 @@
       <c r="E301" t="n">
         <v>63</v>
       </c>
-      <c r="F301" t="inlineStr">
+      <c r="F301" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G301" t="inlineStr">
         <is>
           <t>16/jan</t>
         </is>
@@ -7611,7 +8516,10 @@
       <c r="E302" t="n">
         <v>28</v>
       </c>
-      <c r="F302" t="inlineStr">
+      <c r="F302" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G302" t="inlineStr">
         <is>
           <t>17/jan</t>
         </is>
@@ -7635,7 +8543,10 @@
       <c r="E303" t="n">
         <v>36</v>
       </c>
-      <c r="F303" t="inlineStr">
+      <c r="F303" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G303" t="inlineStr">
         <is>
           <t>18/jan</t>
         </is>
@@ -7659,7 +8570,10 @@
       <c r="E304" t="n">
         <v>19</v>
       </c>
-      <c r="F304" t="inlineStr">
+      <c r="F304" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G304" t="inlineStr">
         <is>
           <t>19/jan</t>
         </is>
@@ -7683,7 +8597,10 @@
       <c r="E305" t="n">
         <v>39</v>
       </c>
-      <c r="F305" t="inlineStr">
+      <c r="F305" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G305" t="inlineStr">
         <is>
           <t>20/jan</t>
         </is>
@@ -7707,7 +8624,10 @@
       <c r="E306" t="n">
         <v>26</v>
       </c>
-      <c r="F306" t="inlineStr">
+      <c r="F306" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G306" t="inlineStr">
         <is>
           <t>21/jan</t>
         </is>
@@ -7731,7 +8651,10 @@
       <c r="E307" t="n">
         <v>41</v>
       </c>
-      <c r="F307" t="inlineStr">
+      <c r="F307" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G307" t="inlineStr">
         <is>
           <t>22/jan</t>
         </is>
@@ -7755,7 +8678,10 @@
       <c r="E308" t="n">
         <v>46</v>
       </c>
-      <c r="F308" t="inlineStr">
+      <c r="F308" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G308" t="inlineStr">
         <is>
           <t>23/jan</t>
         </is>
@@ -7779,7 +8705,10 @@
       <c r="E309" t="n">
         <v>36</v>
       </c>
-      <c r="F309" t="inlineStr">
+      <c r="F309" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G309" t="inlineStr">
         <is>
           <t>24/jan</t>
         </is>
@@ -7803,7 +8732,10 @@
       <c r="E310" t="n">
         <v>13</v>
       </c>
-      <c r="F310" t="inlineStr">
+      <c r="F310" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G310" t="inlineStr">
         <is>
           <t>25/jan</t>
         </is>
@@ -7827,7 +8759,10 @@
       <c r="E311" t="n">
         <v>17</v>
       </c>
-      <c r="F311" t="inlineStr">
+      <c r="F311" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G311" t="inlineStr">
         <is>
           <t>26/jan</t>
         </is>
@@ -7851,7 +8786,10 @@
       <c r="E312" t="n">
         <v>70</v>
       </c>
-      <c r="F312" t="inlineStr">
+      <c r="F312" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G312" t="inlineStr">
         <is>
           <t>27/jan</t>
         </is>
@@ -7875,7 +8813,10 @@
       <c r="E313" t="n">
         <v>50</v>
       </c>
-      <c r="F313" t="inlineStr">
+      <c r="F313" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G313" t="inlineStr">
         <is>
           <t>28/jan</t>
         </is>
@@ -7899,7 +8840,10 @@
       <c r="E314" t="n">
         <v>62</v>
       </c>
-      <c r="F314" t="inlineStr">
+      <c r="F314" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G314" t="inlineStr">
         <is>
           <t>29/jan</t>
         </is>
@@ -7923,7 +8867,10 @@
       <c r="E315" t="n">
         <v>48</v>
       </c>
-      <c r="F315" t="inlineStr">
+      <c r="F315" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G315" t="inlineStr">
         <is>
           <t>30/jan</t>
         </is>
@@ -7947,7 +8894,10 @@
       <c r="E316" t="n">
         <v>39</v>
       </c>
-      <c r="F316" t="inlineStr">
+      <c r="F316" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G316" t="inlineStr">
         <is>
           <t>31/jan</t>
         </is>
@@ -7971,7 +8921,10 @@
       <c r="E317" t="n">
         <v>5</v>
       </c>
-      <c r="F317" t="inlineStr">
+      <c r="F317" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G317" t="inlineStr">
         <is>
           <t>01/fev</t>
         </is>
@@ -7995,7 +8948,10 @@
       <c r="E318" t="n">
         <v>19</v>
       </c>
-      <c r="F318" t="inlineStr">
+      <c r="F318" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G318" t="inlineStr">
         <is>
           <t>02/fev</t>
         </is>
@@ -8019,7 +8975,10 @@
       <c r="E319" t="n">
         <v>43</v>
       </c>
-      <c r="F319" t="inlineStr">
+      <c r="F319" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G319" t="inlineStr">
         <is>
           <t>03/fev</t>
         </is>
@@ -8043,7 +9002,10 @@
       <c r="E320" t="n">
         <v>45</v>
       </c>
-      <c r="F320" t="inlineStr">
+      <c r="F320" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G320" t="inlineStr">
         <is>
           <t>04/fev</t>
         </is>
@@ -8067,7 +9029,10 @@
       <c r="E321" t="n">
         <v>51</v>
       </c>
-      <c r="F321" t="inlineStr">
+      <c r="F321" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G321" t="inlineStr">
         <is>
           <t>05/fev</t>
         </is>
@@ -8091,7 +9056,10 @@
       <c r="E322" t="n">
         <v>30</v>
       </c>
-      <c r="F322" t="inlineStr">
+      <c r="F322" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G322" t="inlineStr">
         <is>
           <t>06/fev</t>
         </is>
@@ -8115,7 +9083,10 @@
       <c r="E323" t="n">
         <v>20</v>
       </c>
-      <c r="F323" t="inlineStr">
+      <c r="F323" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G323" t="inlineStr">
         <is>
           <t>07/fev</t>
         </is>
@@ -8139,7 +9110,10 @@
       <c r="E324" t="n">
         <v>7</v>
       </c>
-      <c r="F324" t="inlineStr">
+      <c r="F324" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G324" t="inlineStr">
         <is>
           <t>08/fev</t>
         </is>
@@ -8163,7 +9137,10 @@
       <c r="E325" t="n">
         <v>25</v>
       </c>
-      <c r="F325" t="inlineStr">
+      <c r="F325" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G325" t="inlineStr">
         <is>
           <t>09/fev</t>
         </is>
@@ -8187,7 +9164,10 @@
       <c r="E326" t="n">
         <v>39</v>
       </c>
-      <c r="F326" t="inlineStr">
+      <c r="F326" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G326" t="inlineStr">
         <is>
           <t>10/fev</t>
         </is>
@@ -8211,7 +9191,10 @@
       <c r="E327" t="n">
         <v>28</v>
       </c>
-      <c r="F327" t="inlineStr">
+      <c r="F327" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G327" t="inlineStr">
         <is>
           <t>11/fev</t>
         </is>
@@ -8235,7 +9218,10 @@
       <c r="E328" t="n">
         <v>43</v>
       </c>
-      <c r="F328" t="inlineStr">
+      <c r="F328" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G328" t="inlineStr">
         <is>
           <t>12/fev</t>
         </is>
@@ -8259,7 +9245,10 @@
       <c r="E329" t="n">
         <v>32</v>
       </c>
-      <c r="F329" t="inlineStr">
+      <c r="F329" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G329" t="inlineStr">
         <is>
           <t>13/fev</t>
         </is>
@@ -8283,7 +9272,10 @@
       <c r="E330" t="n">
         <v>18</v>
       </c>
-      <c r="F330" t="inlineStr">
+      <c r="F330" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G330" t="inlineStr">
         <is>
           <t>14/fev</t>
         </is>
@@ -8307,7 +9299,10 @@
       <c r="E331" t="n">
         <v>15</v>
       </c>
-      <c r="F331" t="inlineStr">
+      <c r="F331" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G331" t="inlineStr">
         <is>
           <t>15/fev</t>
         </is>
@@ -8331,7 +9326,10 @@
       <c r="E332" t="n">
         <v>26</v>
       </c>
-      <c r="F332" t="inlineStr">
+      <c r="F332" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G332" t="inlineStr">
         <is>
           <t>16/fev</t>
         </is>
@@ -8355,7 +9353,10 @@
       <c r="E333" t="n">
         <v>58</v>
       </c>
-      <c r="F333" t="inlineStr">
+      <c r="F333" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G333" t="inlineStr">
         <is>
           <t>17/fev</t>
         </is>
@@ -8379,7 +9380,10 @@
       <c r="E334" t="n">
         <v>30</v>
       </c>
-      <c r="F334" t="inlineStr">
+      <c r="F334" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G334" t="inlineStr">
         <is>
           <t>18/fev</t>
         </is>
@@ -8403,7 +9407,10 @@
       <c r="E335" t="n">
         <v>53</v>
       </c>
-      <c r="F335" t="inlineStr">
+      <c r="F335" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G335" t="inlineStr">
         <is>
           <t>19/fev</t>
         </is>
@@ -8427,7 +9434,10 @@
       <c r="E336" t="n">
         <v>44</v>
       </c>
-      <c r="F336" t="inlineStr">
+      <c r="F336" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G336" t="inlineStr">
         <is>
           <t>20/fev</t>
         </is>
@@ -8451,7 +9461,10 @@
       <c r="E337" t="n">
         <v>37</v>
       </c>
-      <c r="F337" t="inlineStr">
+      <c r="F337" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G337" t="inlineStr">
         <is>
           <t>21/fev</t>
         </is>
@@ -8475,7 +9488,10 @@
       <c r="E338" t="n">
         <v>13</v>
       </c>
-      <c r="F338" t="inlineStr">
+      <c r="F338" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G338" t="inlineStr">
         <is>
           <t>22/fev</t>
         </is>
@@ -8499,7 +9515,10 @@
       <c r="E339" t="n">
         <v>24</v>
       </c>
-      <c r="F339" t="inlineStr">
+      <c r="F339" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G339" t="inlineStr">
         <is>
           <t>23/fev</t>
         </is>
@@ -8523,7 +9542,10 @@
       <c r="E340" t="n">
         <v>37</v>
       </c>
-      <c r="F340" t="inlineStr">
+      <c r="F340" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G340" t="inlineStr">
         <is>
           <t>24/fev</t>
         </is>
@@ -8547,7 +9569,10 @@
       <c r="E341" t="n">
         <v>36</v>
       </c>
-      <c r="F341" t="inlineStr">
+      <c r="F341" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G341" t="inlineStr">
         <is>
           <t>25/fev</t>
         </is>
@@ -8571,7 +9596,10 @@
       <c r="E342" t="n">
         <v>50</v>
       </c>
-      <c r="F342" t="inlineStr">
+      <c r="F342" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G342" t="inlineStr">
         <is>
           <t>26/fev</t>
         </is>
@@ -8595,7 +9623,10 @@
       <c r="E343" t="n">
         <v>75</v>
       </c>
-      <c r="F343" t="inlineStr">
+      <c r="F343" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G343" t="inlineStr">
         <is>
           <t>27/fev</t>
         </is>
@@ -8619,7 +9650,10 @@
       <c r="E344" t="n">
         <v>16</v>
       </c>
-      <c r="F344" t="inlineStr">
+      <c r="F344" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G344" t="inlineStr">
         <is>
           <t>28/fev</t>
         </is>
@@ -8643,7 +9677,10 @@
       <c r="E345" t="n">
         <v>6</v>
       </c>
-      <c r="F345" t="inlineStr">
+      <c r="F345" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G345" t="inlineStr">
         <is>
           <t>01/mar</t>
         </is>
@@ -8667,7 +9704,10 @@
       <c r="E346" t="n">
         <v>41</v>
       </c>
-      <c r="F346" t="inlineStr">
+      <c r="F346" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G346" t="inlineStr">
         <is>
           <t>02/mar</t>
         </is>
@@ -8691,7 +9731,10 @@
       <c r="E347" t="n">
         <v>55</v>
       </c>
-      <c r="F347" t="inlineStr">
+      <c r="F347" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G347" t="inlineStr">
         <is>
           <t>03/mar</t>
         </is>
@@ -8715,7 +9758,10 @@
       <c r="E348" t="n">
         <v>67</v>
       </c>
-      <c r="F348" t="inlineStr">
+      <c r="F348" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G348" t="inlineStr">
         <is>
           <t>04/mar</t>
         </is>
@@ -8739,7 +9785,10 @@
       <c r="E349" t="n">
         <v>128</v>
       </c>
-      <c r="F349" t="inlineStr">
+      <c r="F349" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G349" t="inlineStr">
         <is>
           <t>05/mar</t>
         </is>
@@ -8763,7 +9812,10 @@
       <c r="E350" t="n">
         <v>86</v>
       </c>
-      <c r="F350" t="inlineStr">
+      <c r="F350" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G350" t="inlineStr">
         <is>
           <t>06/mar</t>
         </is>
@@ -8787,7 +9839,10 @@
       <c r="E351" t="n">
         <v>23</v>
       </c>
-      <c r="F351" t="inlineStr">
+      <c r="F351" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G351" t="inlineStr">
         <is>
           <t>07/mar</t>
         </is>
@@ -8811,7 +9866,10 @@
       <c r="E352" t="n">
         <v>25</v>
       </c>
-      <c r="F352" t="inlineStr">
+      <c r="F352" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G352" t="inlineStr">
         <is>
           <t>08/mar</t>
         </is>
@@ -8835,7 +9893,10 @@
       <c r="E353" t="n">
         <v>37</v>
       </c>
-      <c r="F353" t="inlineStr">
+      <c r="F353" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G353" t="inlineStr">
         <is>
           <t>09/mar</t>
         </is>
@@ -8859,7 +9920,10 @@
       <c r="E354" t="n">
         <v>113</v>
       </c>
-      <c r="F354" t="inlineStr">
+      <c r="F354" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G354" t="inlineStr">
         <is>
           <t>10/mar</t>
         </is>
@@ -8883,7 +9947,10 @@
       <c r="E355" t="n">
         <v>85</v>
       </c>
-      <c r="F355" t="inlineStr">
+      <c r="F355" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G355" t="inlineStr">
         <is>
           <t>11/mar</t>
         </is>
@@ -8907,7 +9974,10 @@
       <c r="E356" t="n">
         <v>0</v>
       </c>
-      <c r="F356" t="inlineStr">
+      <c r="F356" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G356" t="inlineStr">
         <is>
           <t>12/mar</t>
         </is>
@@ -8931,7 +10001,10 @@
       <c r="E357" t="n">
         <v>0</v>
       </c>
-      <c r="F357" t="inlineStr">
+      <c r="F357" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G357" t="inlineStr">
         <is>
           <t>13/mar</t>
         </is>
@@ -8955,7 +10028,10 @@
       <c r="E358" t="n">
         <v>0</v>
       </c>
-      <c r="F358" t="inlineStr">
+      <c r="F358" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G358" t="inlineStr">
         <is>
           <t>14/mar</t>
         </is>
@@ -8979,7 +10055,10 @@
       <c r="E359" t="n">
         <v>236</v>
       </c>
-      <c r="F359" t="inlineStr">
+      <c r="F359" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G359" t="inlineStr">
         <is>
           <t>15/mar</t>
         </is>
@@ -9003,7 +10082,10 @@
       <c r="E360" t="n">
         <v>47</v>
       </c>
-      <c r="F360" t="inlineStr">
+      <c r="F360" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G360" t="inlineStr">
         <is>
           <t>16/mar</t>
         </is>
@@ -9016,20 +10098,104 @@
         </is>
       </c>
       <c r="B361" t="n">
-        <v>10715</v>
+        <v>10834</v>
       </c>
       <c r="C361" t="n">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D361" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E361" t="n">
-        <v>0</v>
-      </c>
-      <c r="F361" t="inlineStr">
+        <v>119</v>
+      </c>
+      <c r="F361" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G361" t="inlineStr">
         <is>
           <t>17/mar</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" s="1" t="inlineStr">
+        <is>
+          <t>18/mar</t>
+        </is>
+      </c>
+      <c r="B362" t="n">
+        <v>10834</v>
+      </c>
+      <c r="C362" t="n">
+        <v>190</v>
+      </c>
+      <c r="D362" t="n">
+        <v>0</v>
+      </c>
+      <c r="E362" t="n">
+        <v>0</v>
+      </c>
+      <c r="F362" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G362" t="inlineStr">
+        <is>
+          <t>18/mar</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" s="1" t="inlineStr">
+        <is>
+          <t>19/mar</t>
+        </is>
+      </c>
+      <c r="B363" t="n">
+        <v>11011</v>
+      </c>
+      <c r="C363" t="n">
+        <v>197</v>
+      </c>
+      <c r="D363" t="n">
+        <v>7</v>
+      </c>
+      <c r="E363" t="n">
+        <v>177</v>
+      </c>
+      <c r="F363" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G363" t="inlineStr">
+        <is>
+          <t>19/mar</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" s="1" t="inlineStr">
+        <is>
+          <t>20/mar</t>
+        </is>
+      </c>
+      <c r="B364" t="n">
+        <v>11011</v>
+      </c>
+      <c r="C364" t="n">
+        <v>197</v>
+      </c>
+      <c r="D364" t="n">
+        <v>0</v>
+      </c>
+      <c r="E364" t="n">
+        <v>0</v>
+      </c>
+      <c r="F364" t="n">
+        <v>218162</v>
+      </c>
+      <c r="G364" t="inlineStr">
+        <is>
+          <t>20/mar</t>
         </is>
       </c>
     </row>

</xml_diff>